<commit_message>
Revamped Transaction consensus, working on 20-node functionality
</commit_message>
<xml_diff>
--- a/Storage/B_visualization.xlsx
+++ b/Storage/B_visualization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spaul/Documents/BlockchainTest/Storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A1031F-8032-4045-A402-20AE161BFBA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9483390A-02CB-3846-AEAE-46350D2F9A58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11200" yWindow="1540" windowWidth="28040" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="balances" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>index</t>
   </si>
   <si>
-    <t>653c2ebdd7f612544dd6e1aae2f00d5d3fb77a7bc9d1e705ab2c3efaa5ec848e</t>
+    <t>c396ef5e0d3b2fdb947efd81e28755c46fe9ed8df31f76c0e86e5dd3770d5494</t>
   </si>
   <si>
-    <t>3836fab125046e9ba4c0ecb377caccc9b5b4294ce93872c995c2174455eb9024</t>
+    <t>bb92bdbb2e83542aefa863f78dd7b5b3dcfbcc4690299637538b14d73eb5439d</t>
   </si>
   <si>
-    <t>af6b891023b03f5ed36c0e97266b2fcf8c4826462b97ca8cec8e4e85c93f4510</t>
+    <t>162d0c262288952f87f67b195438d368c71ade6a92fe647eb191b40b59855dd1</t>
   </si>
   <si>
-    <t>c2e9f6d78d4f264882728ea780ed67584734c638c4061d6d4733ea79d8a1d3df</t>
+    <t>923b912a0b971c7959af6b958321c527f5d628c2ae0e7fb1c005810109ba223f</t>
+  </si>
+  <si>
+    <t>99fb3577ddfad19d53747ac9b1c89ded87a27176adf0e7218b60891110a8f05e</t>
+  </si>
+  <si>
+    <t>ba387a009d3eb1e8a9ac56dd395e8ee230bd5035122ce908f86bd9c8d67271a0</t>
+  </si>
+  <si>
+    <t>66e931ef8387b569d6435361bc4e77ff6629b66dc04802cb7aa210a5852a5178</t>
+  </si>
+  <si>
+    <t>9e6f221da29e0125a2c0da7862f9ebd35f4b5aa8a34a1d97b2de8b07e308668e</t>
+  </si>
+  <si>
+    <t>c6f523cf1df00f9e23c8bda3495300d6afdefc6746c27dd342238a4dd102ca82</t>
+  </si>
+  <si>
+    <t>6d0a3e622e1f44cb359f0fadc5abcedfd735f08f7f7efe518fe7152e4734b807</t>
   </si>
 </sst>
 </file>
@@ -518,8 +536,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -643,122 +662,122 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>balances!$A$2:$A$42</c:f>
+              <c:f>balances!$B$2:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>37</c:v>
@@ -770,139 +789,13 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>balances!$B$2:$B$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="32">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>45</c:v>
+                <c:pt idx="41">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,7 +803,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4ECD-7848-A920-7D4DB9D702F7}"/>
+              <c16:uniqueId val="{00000000-43CD-DF42-99CC-0716850F964D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -929,144 +822,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>balances!$A$2:$A$42</c:f>
+              <c:f>balances!$C$2:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>balances!$C$2:$C$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1074,43 +835,43 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>30</c:v>
@@ -1119,76 +880,82 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="26">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="28">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="30">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>45</c:v>
+                <c:pt idx="41">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1196,7 +963,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4ECD-7848-A920-7D4DB9D702F7}"/>
+              <c16:uniqueId val="{00000001-43CD-DF42-99CC-0716850F964D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1215,144 +982,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>balances!$A$2:$A$42</c:f>
+              <c:f>balances!$D$2:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>balances!$D$2:$D$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1360,28 +995,28 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>26</c:v>
@@ -1390,28 +1025,28 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>34</c:v>
@@ -1420,34 +1055,34 @@
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>34</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>35</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>35</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>36</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>37</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>38</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>38</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>39</c:v>
@@ -1456,25 +1091,31 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>42</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>43</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>44</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1482,7 +1123,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4ECD-7848-A920-7D4DB9D702F7}"/>
+              <c16:uniqueId val="{00000002-43CD-DF42-99CC-0716850F964D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1501,144 +1142,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>balances!$A$2:$A$42</c:f>
+              <c:f>balances!$E$2:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>balances!$E$2:$E$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1655,10 +1164,10 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>23</c:v>
@@ -1667,100 +1176,106 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="19">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="21">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="22">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="23">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="24">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="25">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="26">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="28">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="35">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="36">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="37">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="38">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="39">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="40">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="38">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>46</c:v>
+                <c:pt idx="41">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,7 +1283,975 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-4ECD-7848-A920-7D4DB9D702F7}"/>
+              <c16:uniqueId val="{00000003-43CD-DF42-99CC-0716850F964D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>balances!$F$2:$F$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-43CD-DF42-99CC-0716850F964D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>balances!$G$2:$G$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-43CD-DF42-99CC-0716850F964D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>balances!$H$2:$H$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-43CD-DF42-99CC-0716850F964D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>balances!$I$2:$I$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-43CD-DF42-99CC-0716850F964D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>balances!$J$2:$J$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-43CD-DF42-99CC-0716850F964D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>balances!$K$2:$K$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-43CD-DF42-99CC-0716850F964D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1781,17 +2264,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1510389248"/>
-        <c:axId val="1510402768"/>
+        <c:axId val="1695491423"/>
+        <c:axId val="1695518015"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1510389248"/>
+        <c:axId val="1695491423"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1809,7 +2291,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1828,7 +2310,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1510402768"/>
+        <c:crossAx val="1695518015"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1836,7 +2318,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1510402768"/>
+        <c:axId val="1695518015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1887,7 +2369,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1510389248"/>
+        <c:crossAx val="1695491423"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2534,23 +3016,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAA7B3DC-790D-EC4A-8050-A8C1A7C3688E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03C196AE-0D96-054E-A5AC-0AA1B5BE15FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2868,15 +3350,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2892,8 +3374,26 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2909,8 +3409,26 @@
       <c r="E2">
         <v>20</v>
       </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2926,25 +3444,61 @@
       <c r="E3">
         <v>20</v>
       </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4">
         <v>20</v>
-      </c>
-      <c r="D4">
-        <v>21</v>
       </c>
       <c r="E4">
         <v>21</v>
       </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2952,7 +3506,7 @@
         <v>22</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>21</v>
@@ -2960,8 +3514,26 @@
       <c r="E5">
         <v>22</v>
       </c>
+      <c r="F5">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>21</v>
+      </c>
+      <c r="H5">
+        <v>21</v>
+      </c>
+      <c r="I5">
+        <v>21</v>
+      </c>
+      <c r="J5">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2969,16 +3541,34 @@
         <v>22</v>
       </c>
       <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
         <v>21</v>
-      </c>
-      <c r="D6">
-        <v>22</v>
       </c>
       <c r="E6">
         <v>22</v>
       </c>
+      <c r="F6">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>22</v>
+      </c>
+      <c r="J6">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2986,16 +3576,34 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <v>22</v>
+      </c>
+      <c r="I7">
+        <v>22</v>
+      </c>
+      <c r="J7">
         <v>23</v>
       </c>
-      <c r="E7">
-        <v>23</v>
+      <c r="K7">
+        <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3003,16 +3611,34 @@
         <v>24</v>
       </c>
       <c r="C8">
+        <v>23</v>
+      </c>
+      <c r="D8">
         <v>22</v>
       </c>
-      <c r="D8">
-        <v>24</v>
-      </c>
       <c r="E8">
+        <v>22</v>
+      </c>
+      <c r="F8">
         <v>23</v>
       </c>
+      <c r="G8">
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <v>23</v>
+      </c>
+      <c r="I8">
+        <v>23</v>
+      </c>
+      <c r="J8">
+        <v>23</v>
+      </c>
+      <c r="K8">
+        <v>25</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3020,50 +3646,104 @@
         <v>25</v>
       </c>
       <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
         <v>23</v>
-      </c>
-      <c r="D9">
-        <v>25</v>
       </c>
       <c r="E9">
         <v>23</v>
       </c>
+      <c r="F9">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>22</v>
+      </c>
+      <c r="H9">
+        <v>24</v>
+      </c>
+      <c r="I9">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>24</v>
+      </c>
+      <c r="K9">
+        <v>25</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
+        <v>26</v>
+      </c>
+      <c r="C10">
         <v>25</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>24</v>
-      </c>
-      <c r="D10">
-        <v>26</v>
       </c>
       <c r="E10">
         <v>24</v>
       </c>
+      <c r="F10">
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <v>23</v>
+      </c>
+      <c r="H10">
+        <v>25</v>
+      </c>
+      <c r="I10">
+        <v>25</v>
+      </c>
+      <c r="J10">
+        <v>25</v>
+      </c>
+      <c r="K10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11">
         <v>25</v>
       </c>
-      <c r="C11">
+      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="F11">
         <v>25</v>
       </c>
-      <c r="D11">
+      <c r="G11">
+        <v>23</v>
+      </c>
+      <c r="H11">
+        <v>25</v>
+      </c>
+      <c r="I11">
+        <v>25</v>
+      </c>
+      <c r="J11">
+        <v>25</v>
+      </c>
+      <c r="K11">
         <v>26</v>
       </c>
-      <c r="E11">
-        <v>25</v>
-      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3071,271 +3751,559 @@
         <v>26</v>
       </c>
       <c r="C12">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <v>26</v>
       </c>
       <c r="E12">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <v>26</v>
+      </c>
+      <c r="G12">
+        <v>23</v>
+      </c>
+      <c r="H12">
         <v>25</v>
       </c>
+      <c r="I12">
+        <v>26</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>26</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>27</v>
       </c>
       <c r="E13">
+        <v>24</v>
+      </c>
+      <c r="F13">
         <v>26</v>
       </c>
+      <c r="G13">
+        <v>24</v>
+      </c>
+      <c r="H13">
+        <v>25</v>
+      </c>
+      <c r="I13">
+        <v>27</v>
+      </c>
+      <c r="J13">
+        <v>25</v>
+      </c>
+      <c r="K13">
+        <v>26</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <v>25</v>
+      </c>
+      <c r="F14">
         <v>26</v>
       </c>
-      <c r="C14">
+      <c r="G14">
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <v>26</v>
+      </c>
+      <c r="I14">
         <v>27</v>
       </c>
-      <c r="D14">
-        <v>28</v>
-      </c>
-      <c r="E14">
-        <v>27</v>
+      <c r="J14">
+        <v>26</v>
+      </c>
+      <c r="K14">
+        <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
+      </c>
+      <c r="E15">
         <v>26</v>
       </c>
-      <c r="C15">
+      <c r="F15">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>25</v>
+      </c>
+      <c r="H15">
+        <v>27</v>
+      </c>
+      <c r="I15">
         <v>28</v>
       </c>
-      <c r="D15">
-        <v>29</v>
-      </c>
-      <c r="E15">
-        <v>28</v>
+      <c r="J15">
+        <v>27</v>
+      </c>
+      <c r="K15">
+        <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>29</v>
+      </c>
+      <c r="E16">
         <v>26</v>
       </c>
-      <c r="C16">
+      <c r="F16">
+        <v>26</v>
+      </c>
+      <c r="G16">
+        <v>25</v>
+      </c>
+      <c r="H16">
+        <v>27</v>
+      </c>
+      <c r="I16">
         <v>29</v>
       </c>
-      <c r="D16">
-        <v>30</v>
-      </c>
-      <c r="E16">
-        <v>29</v>
+      <c r="J16">
+        <v>27</v>
+      </c>
+      <c r="K16">
+        <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>30</v>
       </c>
       <c r="D17">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="F17">
+        <v>26</v>
+      </c>
+      <c r="G17">
+        <v>25</v>
+      </c>
+      <c r="H17">
+        <v>27</v>
+      </c>
+      <c r="I17">
+        <v>29</v>
+      </c>
+      <c r="J17">
+        <v>27</v>
+      </c>
+      <c r="K17">
+        <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <v>30</v>
       </c>
       <c r="D18">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="F18">
+        <v>27</v>
+      </c>
+      <c r="G18">
+        <v>26</v>
+      </c>
+      <c r="H18">
+        <v>28</v>
+      </c>
+      <c r="I18">
+        <v>29</v>
+      </c>
+      <c r="J18">
+        <v>27</v>
+      </c>
+      <c r="K18">
+        <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>31</v>
+      </c>
+      <c r="E19">
         <v>28</v>
       </c>
-      <c r="C19">
-        <v>31</v>
-      </c>
-      <c r="D19">
-        <v>33</v>
-      </c>
-      <c r="E19">
-        <v>31</v>
+      <c r="F19">
+        <v>28</v>
+      </c>
+      <c r="G19">
+        <v>26</v>
+      </c>
+      <c r="H19">
+        <v>28</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+      <c r="J19">
+        <v>28</v>
+      </c>
+      <c r="K19">
+        <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20">
         <v>32</v>
       </c>
-      <c r="D20">
-        <v>33</v>
-      </c>
       <c r="E20">
+        <v>29</v>
+      </c>
+      <c r="F20">
+        <v>29</v>
+      </c>
+      <c r="G20">
+        <v>27</v>
+      </c>
+      <c r="H20">
+        <v>29</v>
+      </c>
+      <c r="I20">
         <v>31</v>
       </c>
+      <c r="J20">
+        <v>29</v>
+      </c>
+      <c r="K20">
+        <v>29</v>
+      </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>33</v>
+      </c>
+      <c r="E21">
         <v>29</v>
       </c>
-      <c r="C21">
+      <c r="F21">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>27</v>
+      </c>
+      <c r="H21">
+        <v>30</v>
+      </c>
+      <c r="I21">
         <v>32</v>
       </c>
-      <c r="D21">
-        <v>34</v>
-      </c>
-      <c r="E21">
-        <v>32</v>
+      <c r="J21">
+        <v>30</v>
+      </c>
+      <c r="K21">
+        <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C22">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22">
         <v>34</v>
       </c>
       <c r="E22">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="F22">
+        <v>31</v>
+      </c>
+      <c r="G22">
+        <v>28</v>
+      </c>
+      <c r="H22">
+        <v>31</v>
+      </c>
+      <c r="I22">
+        <v>33</v>
+      </c>
+      <c r="J22">
+        <v>31</v>
+      </c>
+      <c r="K22">
+        <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C23">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23">
         <v>34</v>
       </c>
       <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <v>31</v>
+      </c>
+      <c r="G23">
+        <v>29</v>
+      </c>
+      <c r="H23">
+        <v>31</v>
+      </c>
+      <c r="I23">
         <v>33</v>
       </c>
+      <c r="J23">
+        <v>31</v>
+      </c>
+      <c r="K23">
+        <v>32</v>
+      </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>31</v>
+      </c>
+      <c r="D24">
+        <v>35</v>
+      </c>
+      <c r="E24">
+        <v>31</v>
+      </c>
+      <c r="F24">
+        <v>32</v>
+      </c>
+      <c r="G24">
         <v>30</v>
       </c>
-      <c r="C24">
+      <c r="H24">
+        <v>32</v>
+      </c>
+      <c r="I24">
         <v>34</v>
       </c>
-      <c r="D24">
-        <v>34</v>
-      </c>
-      <c r="E24">
-        <v>34</v>
+      <c r="J24">
+        <v>32</v>
+      </c>
+      <c r="K24">
+        <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
+        <v>33</v>
+      </c>
+      <c r="C25">
         <v>31</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>35</v>
       </c>
-      <c r="D25">
+      <c r="E25">
+        <v>31</v>
+      </c>
+      <c r="F25">
+        <v>32</v>
+      </c>
+      <c r="G25">
+        <v>31</v>
+      </c>
+      <c r="H25">
+        <v>32</v>
+      </c>
+      <c r="I25">
         <v>34</v>
       </c>
-      <c r="E25">
-        <v>34</v>
+      <c r="J25">
+        <v>32</v>
+      </c>
+      <c r="K25">
+        <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>36</v>
+      </c>
+      <c r="E26">
         <v>32</v>
       </c>
-      <c r="C26">
+      <c r="F26">
+        <v>32</v>
+      </c>
+      <c r="G26">
+        <v>32</v>
+      </c>
+      <c r="H26">
+        <v>33</v>
+      </c>
+      <c r="I26">
         <v>35</v>
       </c>
-      <c r="D26">
-        <v>34</v>
-      </c>
-      <c r="E26">
-        <v>35</v>
+      <c r="J26">
+        <v>33</v>
+      </c>
+      <c r="K26">
+        <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>36</v>
+      </c>
+      <c r="E27">
         <v>33</v>
       </c>
-      <c r="C27">
-        <v>35</v>
-      </c>
-      <c r="D27">
+      <c r="F27">
+        <v>33</v>
+      </c>
+      <c r="G27">
+        <v>33</v>
+      </c>
+      <c r="H27">
+        <v>33</v>
+      </c>
+      <c r="I27">
+        <v>36</v>
+      </c>
+      <c r="J27">
         <v>34</v>
       </c>
-      <c r="E27">
-        <v>35</v>
+      <c r="K27">
+        <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3343,16 +4311,34 @@
         <v>34</v>
       </c>
       <c r="C28">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>33</v>
+      </c>
+      <c r="F28">
+        <v>34</v>
+      </c>
+      <c r="G28">
+        <v>33</v>
+      </c>
+      <c r="H28">
+        <v>34</v>
+      </c>
+      <c r="I28">
         <v>36</v>
       </c>
-      <c r="D28">
+      <c r="J28">
+        <v>34</v>
+      </c>
+      <c r="K28">
         <v>35</v>
       </c>
-      <c r="E28">
-        <v>36</v>
-      </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3360,234 +4346,556 @@
         <v>35</v>
       </c>
       <c r="C29">
+        <v>34</v>
+      </c>
+      <c r="D29">
+        <v>38</v>
+      </c>
+      <c r="E29">
+        <v>34</v>
+      </c>
+      <c r="F29">
+        <v>35</v>
+      </c>
+      <c r="G29">
+        <v>33</v>
+      </c>
+      <c r="H29">
+        <v>34</v>
+      </c>
+      <c r="I29">
         <v>37</v>
       </c>
-      <c r="D29">
+      <c r="J29">
         <v>35</v>
       </c>
-      <c r="E29">
+      <c r="K29">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30">
+        <v>35</v>
+      </c>
+      <c r="D30">
+        <v>39</v>
+      </c>
+      <c r="E30">
+        <v>35</v>
+      </c>
+      <c r="F30">
+        <v>35</v>
+      </c>
+      <c r="G30">
+        <v>33</v>
+      </c>
+      <c r="H30">
+        <v>35</v>
+      </c>
+      <c r="I30">
         <v>37</v>
       </c>
-      <c r="D30">
-        <v>36</v>
-      </c>
-      <c r="E30">
-        <v>36</v>
+      <c r="J30">
+        <v>35</v>
+      </c>
+      <c r="K30">
+        <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
+        <v>35</v>
+      </c>
+      <c r="C31">
         <v>36</v>
       </c>
-      <c r="C31">
+      <c r="D31">
+        <v>39</v>
+      </c>
+      <c r="E31">
+        <v>36</v>
+      </c>
+      <c r="F31">
+        <v>35</v>
+      </c>
+      <c r="G31">
+        <v>34</v>
+      </c>
+      <c r="H31">
+        <v>35</v>
+      </c>
+      <c r="I31">
         <v>38</v>
       </c>
-      <c r="D31">
+      <c r="J31">
+        <v>35</v>
+      </c>
+      <c r="K31">
         <v>37</v>
       </c>
-      <c r="E31">
-        <v>37</v>
-      </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
+        <v>35</v>
+      </c>
+      <c r="C32">
         <v>37</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>39</v>
       </c>
-      <c r="D32">
-        <v>38</v>
-      </c>
       <c r="E32">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="F32">
+        <v>35</v>
+      </c>
+      <c r="G32">
+        <v>34</v>
+      </c>
+      <c r="H32">
+        <v>36</v>
+      </c>
+      <c r="I32">
+        <v>39</v>
+      </c>
+      <c r="J32">
+        <v>36</v>
+      </c>
+      <c r="K32">
+        <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
+        <v>36</v>
+      </c>
+      <c r="C33">
         <v>38</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>39</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>38</v>
       </c>
-      <c r="E33">
-        <v>39</v>
+      <c r="F33">
+        <v>36</v>
+      </c>
+      <c r="G33">
+        <v>35</v>
+      </c>
+      <c r="H33">
+        <v>37</v>
+      </c>
+      <c r="I33">
+        <v>40</v>
+      </c>
+      <c r="J33">
+        <v>37</v>
+      </c>
+      <c r="K33">
+        <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
+        <v>36</v>
+      </c>
+      <c r="C34">
         <v>39</v>
-      </c>
-      <c r="C34">
-        <v>40</v>
       </c>
       <c r="D34">
         <v>39</v>
       </c>
       <c r="E34">
+        <v>38</v>
+      </c>
+      <c r="F34">
+        <v>37</v>
+      </c>
+      <c r="G34">
+        <v>36</v>
+      </c>
+      <c r="H34">
+        <v>37</v>
+      </c>
+      <c r="I34">
         <v>40</v>
       </c>
+      <c r="J34">
+        <v>37</v>
+      </c>
+      <c r="K34">
+        <v>38</v>
+      </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C35">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35">
         <v>39</v>
       </c>
       <c r="E35">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="F35">
+        <v>37</v>
+      </c>
+      <c r="G35">
+        <v>36</v>
+      </c>
+      <c r="H35">
+        <v>37</v>
+      </c>
+      <c r="I35">
+        <v>40</v>
+      </c>
+      <c r="J35">
+        <v>38</v>
+      </c>
+      <c r="K35">
+        <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>39</v>
+      </c>
+      <c r="D36">
         <v>40</v>
       </c>
-      <c r="C36">
-        <v>41</v>
-      </c>
-      <c r="D36">
+      <c r="E36">
         <v>39</v>
       </c>
-      <c r="E36">
-        <v>42</v>
+      <c r="F36">
+        <v>38</v>
+      </c>
+      <c r="G36">
+        <v>36</v>
+      </c>
+      <c r="H36">
+        <v>37</v>
+      </c>
+      <c r="I36">
+        <v>40</v>
+      </c>
+      <c r="J36">
+        <v>38</v>
+      </c>
+      <c r="K36">
+        <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
+        <v>37</v>
+      </c>
+      <c r="C37">
+        <v>40</v>
+      </c>
+      <c r="D37">
         <v>41</v>
       </c>
-      <c r="C37">
-        <v>42</v>
-      </c>
-      <c r="D37">
+      <c r="E37">
         <v>40</v>
       </c>
-      <c r="E37">
-        <v>42</v>
+      <c r="F37">
+        <v>38</v>
+      </c>
+      <c r="G37">
+        <v>36</v>
+      </c>
+      <c r="H37">
+        <v>38</v>
+      </c>
+      <c r="I37">
+        <v>41</v>
+      </c>
+      <c r="J37">
+        <v>39</v>
+      </c>
+      <c r="K37">
+        <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>41</v>
+      </c>
+      <c r="D38">
         <v>42</v>
       </c>
-      <c r="C38">
-        <v>42</v>
-      </c>
-      <c r="D38">
+      <c r="E38">
         <v>41</v>
       </c>
-      <c r="E38">
-        <v>43</v>
+      <c r="F38">
+        <v>38</v>
+      </c>
+      <c r="G38">
+        <v>37</v>
+      </c>
+      <c r="H38">
+        <v>39</v>
+      </c>
+      <c r="I38">
+        <v>41</v>
+      </c>
+      <c r="J38">
+        <v>40</v>
+      </c>
+      <c r="K38">
+        <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C39">
         <v>42</v>
       </c>
       <c r="D39">
+        <v>43</v>
+      </c>
+      <c r="E39">
         <v>42</v>
       </c>
-      <c r="E39">
-        <v>44</v>
+      <c r="F39">
+        <v>39</v>
+      </c>
+      <c r="G39">
+        <v>38</v>
+      </c>
+      <c r="H39">
+        <v>39</v>
+      </c>
+      <c r="I39">
+        <v>41</v>
+      </c>
+      <c r="J39">
+        <v>41</v>
+      </c>
+      <c r="K39">
+        <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C40">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E40">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="F40">
+        <v>39</v>
+      </c>
+      <c r="G40">
+        <v>39</v>
+      </c>
+      <c r="H40">
+        <v>40</v>
+      </c>
+      <c r="I40">
+        <v>42</v>
+      </c>
+      <c r="J40">
+        <v>42</v>
+      </c>
+      <c r="K40">
+        <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C41">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D41">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E41">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F41">
+        <v>40</v>
+      </c>
+      <c r="G41">
+        <v>40</v>
+      </c>
+      <c r="H41">
+        <v>41</v>
+      </c>
+      <c r="I41">
+        <v>43</v>
+      </c>
+      <c r="J41">
+        <v>43</v>
+      </c>
+      <c r="K41">
+        <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
+        <v>39</v>
+      </c>
+      <c r="C42">
+        <v>43</v>
+      </c>
+      <c r="D42">
+        <v>46</v>
+      </c>
+      <c r="E42">
+        <v>44</v>
+      </c>
+      <c r="F42">
+        <v>41</v>
+      </c>
+      <c r="G42">
+        <v>41</v>
+      </c>
+      <c r="H42">
+        <v>42</v>
+      </c>
+      <c r="I42">
+        <v>44</v>
+      </c>
+      <c r="J42">
+        <v>44</v>
+      </c>
+      <c r="K42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>39</v>
+      </c>
+      <c r="C43">
+        <v>43</v>
+      </c>
+      <c r="D43">
+        <v>46</v>
+      </c>
+      <c r="E43">
+        <v>44</v>
+      </c>
+      <c r="F43">
+        <v>41</v>
+      </c>
+      <c r="G43">
+        <v>41</v>
+      </c>
+      <c r="H43">
+        <v>42</v>
+      </c>
+      <c r="I43">
+        <v>44</v>
+      </c>
+      <c r="J43">
         <v>45</v>
       </c>
-      <c r="C42">
+      <c r="K43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>39</v>
+      </c>
+      <c r="C44">
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <v>47</v>
+      </c>
+      <c r="E44">
+        <v>44</v>
+      </c>
+      <c r="F44">
+        <v>41</v>
+      </c>
+      <c r="G44">
+        <v>42</v>
+      </c>
+      <c r="H44">
+        <v>43</v>
+      </c>
+      <c r="I44">
         <v>45</v>
       </c>
-      <c r="D42">
-        <v>44</v>
-      </c>
-      <c r="E42">
-        <v>46</v>
+      <c r="J44">
+        <v>45</v>
+      </c>
+      <c r="K44">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>